<commit_message>
Edit RTMF for freight HDV to be freight logistics/eliminated trips
</commit_message>
<xml_diff>
--- a/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
+++ b/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\trans\RTMF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-us\InputData\trans\RTMF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE4D269-1906-40C9-9438-66386A9FA2BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="2250" windowWidth="23595" windowHeight="14160" xr2:uid="{B1321729-65FD-4E39-A16A-F420F6CD402A}"/>
+    <workbookView xWindow="3930" yWindow="2250" windowWidth="23595" windowHeight="14160"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="RTMF-passengers" sheetId="2" r:id="rId2"/>
     <sheet name="RTMF-freight" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -147,7 +146,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -529,22 +528,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4A295D-ACEE-40E1-A0AB-57EEA1BFAA47}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -552,80 +551,80 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>24</v>
@@ -634,7 +633,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
         <v>25</v>
@@ -643,7 +642,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="2"/>
       <c r="B28" s="1" t="s">
         <v>26</v>
@@ -659,7 +658,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5439016C-B89E-42B2-9367-3788A58F3CB4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -667,14 +666,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.59765625" customWidth="1"/>
+    <col min="8" max="8" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -700,7 +699,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -728,7 +727,7 @@
         <v>0.33999999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -756,7 +755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -784,7 +783,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -812,7 +811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -840,7 +839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -868,7 +867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -883,22 +882,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E2AAAC-5DEA-4554-803B-E8EE05A805DF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.59765625" customWidth="1"/>
+    <col min="8" max="8" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -924,7 +925,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -952,7 +953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -966,10 +967,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="4">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="F3" s="4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -977,10 +978,10 @@
       <c r="H3" s="4"/>
       <c r="I3" s="6">
         <f t="shared" ref="I3:I7" si="0">1-SUM(B3:G3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1008,7 +1009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1036,7 +1037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1064,7 +1065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1092,7 +1093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>

</xml_diff>

<commit_message>
Still more input data updates to consolidate Cargo Type (#174)
</commit_message>
<xml_diff>
--- a/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
+++ b/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\trans\RTMF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FB5531-2677-47B7-9AFB-26A3AFDC9591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0238BE5-1C16-410D-BC1D-2991C167FC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21090" yWindow="660" windowWidth="25935" windowHeight="22050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10875" yWindow="195" windowWidth="25935" windowHeight="22050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
   <si>
     <t>RTMF Recipient Transportation Mode Fractions</t>
   </si>
@@ -44,24 +44,6 @@
   </si>
   <si>
     <t>Unit: dimensionless (%)</t>
-  </si>
-  <si>
-    <t>LDVs</t>
-  </si>
-  <si>
-    <t>HDVs</t>
-  </si>
-  <si>
-    <t>aircraft</t>
-  </si>
-  <si>
-    <t>rail</t>
-  </si>
-  <si>
-    <t>ships</t>
-  </si>
-  <si>
-    <t>motorbikes</t>
   </si>
   <si>
     <t>Notes</t>
@@ -240,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -248,6 +230,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,67 +566,67 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -649,39 +634,39 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -695,46 +680,64 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="2" max="13" width="10.5703125" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B2" s="4">
         <v>0</v>
@@ -754,15 +757,33 @@
       <c r="G2" s="4">
         <v>0</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="6">
-        <f>1-SUM(B2:G2)</f>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+      <c r="N2" s="4"/>
+      <c r="O2" s="6">
+        <f>1-SUM(B2:M2)</f>
         <v>0.33999999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -782,15 +803,33 @@
       <c r="G3" s="4">
         <v>0</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="6">
-        <f t="shared" ref="I3:I7" si="0">1-SUM(B3:G3)</f>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0</v>
+      </c>
+      <c r="N3" s="4"/>
+      <c r="O3" s="6">
+        <f t="shared" ref="O3:O13" si="0">1-SUM(B3:M3)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -810,15 +849,33 @@
       <c r="G4" s="4">
         <v>0</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="6">
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4"/>
+      <c r="O4" s="6">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B5" s="4">
         <v>0</v>
@@ -838,15 +895,33 @@
       <c r="G5" s="4">
         <v>0</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="6">
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B6" s="4">
         <v>0</v>
@@ -866,15 +941,33 @@
       <c r="G6" s="4">
         <v>0</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="6">
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4">
+        <v>0</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B7" s="4">
         <v>0</v>
@@ -894,15 +987,33 @@
       <c r="G7" s="4">
         <v>0</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="6">
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4"/>
+      <c r="O7" s="6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B8" s="4">
         <v>0</v>
@@ -922,15 +1033,33 @@
       <c r="G8" s="4">
         <v>0</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="6">
-        <f>1-SUM(B8:G8)</f>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4"/>
+      <c r="O8" s="6">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B9" s="4">
         <v>0</v>
@@ -950,15 +1079,33 @@
       <c r="G9" s="4">
         <v>0</v>
       </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="6">
-        <f>1-SUM(B9:G9)</f>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0</v>
+      </c>
+      <c r="N9" s="4"/>
+      <c r="O9" s="6">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B10" s="4">
         <v>0</v>
@@ -978,15 +1125,33 @@
       <c r="G10" s="4">
         <v>0</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="6">
-        <f>1-SUM(B10:G10)</f>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+      <c r="M10" s="4">
+        <v>0</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="O10" s="6">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B11" s="4">
         <v>0</v>
@@ -1006,15 +1171,33 @@
       <c r="G11" s="4">
         <v>0</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="6">
-        <f>1-SUM(B11:G11)</f>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4"/>
+      <c r="O11" s="6">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B12" s="4">
         <v>0</v>
@@ -1034,15 +1217,33 @@
       <c r="G12" s="4">
         <v>0</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="6">
-        <f>1-SUM(B12:G12)</f>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4"/>
+      <c r="O12" s="6">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B13" s="4">
         <v>0</v>
@@ -1062,9 +1263,27 @@
       <c r="G13" s="4">
         <v>0</v>
       </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="6">
-        <f>1-SUM(B13:G13)</f>
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4"/>
+      <c r="O13" s="6">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update aircraft to rail / virtual mode shifting distribution (#161)
</commit_message>
<xml_diff>
--- a/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
+++ b/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-us\InputData\trans\RTMF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\trans\RTMF\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879C9A3C-65AE-46B7-AAAF-3BEC51FB4A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="2250" windowWidth="23595" windowHeight="14160"/>
+    <workbookView xWindow="12870" yWindow="1470" windowWidth="22500" windowHeight="21135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="RTMF-passengers" sheetId="2" r:id="rId2"/>
     <sheet name="RTMF-freight" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -146,7 +147,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -528,22 +529,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.73046875" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -551,80 +552,80 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>24</v>
@@ -633,7 +634,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
         <v>25</v>
@@ -642,7 +643,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="1" t="s">
         <v>26</v>
@@ -658,7 +659,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
@@ -666,14 +667,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.3984375" customWidth="1"/>
-    <col min="7" max="7" width="11.59765625" customWidth="1"/>
-    <col min="8" max="8" width="9.1328125" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -699,7 +700,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -727,7 +728,7 @@
         <v>0.33999999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -755,7 +756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -769,7 +770,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="4">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="F4" s="4">
         <v>0</v>
@@ -780,10 +781,10 @@
       <c r="H4" s="4"/>
       <c r="I4" s="6">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -811,7 +812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -839,7 +840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -867,7 +868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -882,24 +883,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.3984375" customWidth="1"/>
-    <col min="7" max="7" width="11.59765625" customWidth="1"/>
-    <col min="8" max="8" width="9.1328125" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -925,7 +924,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -953,7 +952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -981,7 +980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1009,7 +1008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1037,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1065,7 +1064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1093,7 +1092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>

</xml_diff>

<commit_message>
Add policy to reduce freight rail transport to NDC scenario
</commit_message>
<xml_diff>
--- a/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
+++ b/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\trans\RTMF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\trans\RTMF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879C9A3C-65AE-46B7-AAAF-3BEC51FB4A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2643F14-5F7F-4432-8B4A-9A19F1481256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12870" yWindow="1470" windowWidth="22500" windowHeight="21135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>RTMF Recipient Transportation Mode Fractions</t>
   </si>
@@ -138,10 +138,16 @@
     <t>goes to a mix of passenger rail and non-motorized/eliminated</t>
   </si>
   <si>
-    <t>goes to a mix of freight rail and freight ships</t>
-  </si>
-  <si>
     <t>the following mode shifts:</t>
+  </si>
+  <si>
+    <t>freight rail</t>
+  </si>
+  <si>
+    <t>goes to reduced VMT, representing freight logistics</t>
+  </si>
+  <si>
+    <t>goes to reduced VMT, representing lower demand for coal transport</t>
   </si>
 </sst>
 </file>
@@ -208,12 +214,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -234,9 +238,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -274,7 +278,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -380,7 +384,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -522,7 +526,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -530,9 +534,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -603,30 +609,26 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-    </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>30</v>
+      <c r="A25" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>24</v>
       </c>
@@ -635,7 +637,6 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
@@ -644,12 +645,19 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
       <c r="B28" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -663,7 +671,7 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -675,7 +683,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -696,7 +704,7 @@
       <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -704,26 +712,25 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
         <v>0.33</v>
       </c>
-      <c r="D2" s="4">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
         <v>0.33</v>
       </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0</v>
-      </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="6">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
         <f>1-SUM(B2:G2)</f>
         <v>0.33999999999999997</v>
       </c>
@@ -732,26 +739,25 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="6">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
         <f t="shared" ref="I3:I7" si="0">1-SUM(B3:G3)</f>
         <v>1</v>
       </c>
@@ -760,26 +766,25 @@
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
         <v>0.25</v>
       </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="6">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
@@ -788,26 +793,25 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="6">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -816,26 +820,25 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4">
-        <v>0</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="6">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -844,38 +847,28 @@
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4">
-        <v>0</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="6">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -887,7 +880,7 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -899,7 +892,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -920,7 +913,7 @@
       <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -928,26 +921,25 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0</v>
-      </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="6">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
         <f>1-SUM(B2:G2)</f>
         <v>1</v>
       </c>
@@ -956,26 +948,25 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="6">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
         <f t="shared" ref="I3:I7" si="0">1-SUM(B3:G3)</f>
         <v>1</v>
       </c>
@@ -984,26 +975,25 @@
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="6">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1012,26 +1002,25 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="6">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1040,26 +1029,25 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4">
-        <v>0</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="6">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -1068,38 +1056,28 @@
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4">
-        <v>0</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="6">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>